<commit_message>
commit suspensions from 00304
</commit_message>
<xml_diff>
--- a/site/assets/Spring 2020 Coach Suspensions.xlsx
+++ b/site/assets/Spring 2020 Coach Suspensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>suspended</t>
   </si>
@@ -98,18 +98,9 @@
     <t>Wrg/no ID#</t>
   </si>
   <si>
-    <t>Brogen</t>
-  </si>
-  <si>
     <t>Shannon</t>
   </si>
   <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Kenny</t>
-  </si>
-  <si>
     <t>Carlini</t>
   </si>
   <si>
@@ -140,12 +131,6 @@
     <t>Mike</t>
   </si>
   <si>
-    <t>Corgliano</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
     <t>Correa</t>
   </si>
   <si>
@@ -164,9 +149,6 @@
     <t>Paul</t>
   </si>
   <si>
-    <t>D'Alessandro</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -194,87 +176,21 @@
     <t>Sean</t>
   </si>
   <si>
-    <t>Garrett</t>
-  </si>
-  <si>
     <t>Hirsch</t>
   </si>
   <si>
-    <t>Jaussi</t>
-  </si>
-  <si>
-    <t>Joeseph</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>scott</t>
-  </si>
-  <si>
-    <t>Kenney</t>
-  </si>
-  <si>
-    <t>Duane</t>
-  </si>
-  <si>
-    <t>Klinger</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Lawrie</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
     <t>Lisinski</t>
   </si>
   <si>
     <t>Tom</t>
   </si>
   <si>
-    <t xml:space="preserve">Long </t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>MacDonald</t>
-  </si>
-  <si>
-    <t>Nicole</t>
-  </si>
-  <si>
-    <t>Maher</t>
-  </si>
-  <si>
-    <t>Pete</t>
-  </si>
-  <si>
     <t>Marr</t>
   </si>
   <si>
     <t>Kristin</t>
   </si>
   <si>
-    <t>Maslin</t>
-  </si>
-  <si>
-    <t>Erik</t>
-  </si>
-  <si>
-    <t>Milligan</t>
-  </si>
-  <si>
-    <t>O'Connor</t>
-  </si>
-  <si>
-    <t>Tim</t>
-  </si>
-  <si>
     <t>Paolone</t>
   </si>
   <si>
@@ -296,9 +212,6 @@
     <t>Arion</t>
   </si>
   <si>
-    <t>Venuto</t>
-  </si>
-  <si>
     <t>Watson</t>
   </si>
   <si>
@@ -323,21 +236,12 @@
     <t>Jake</t>
   </si>
   <si>
-    <t>Kurtz</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
     <t>Palmieri</t>
   </si>
   <si>
     <t>Rocco</t>
   </si>
   <si>
-    <t>Ritti</t>
-  </si>
-  <si>
     <t>Sipple</t>
   </si>
   <si>
@@ -362,22 +266,46 @@
     <t>Abel</t>
   </si>
   <si>
-    <t>Waters</t>
-  </si>
-  <si>
-    <t>Zapien-Torres</t>
-  </si>
-  <si>
     <t>Jonathan</t>
   </si>
   <si>
-    <t>Nicollette</t>
-  </si>
-  <si>
-    <t>Peggy</t>
-  </si>
-  <si>
     <t>Kennedy</t>
+  </si>
+  <si>
+    <t>Brogan</t>
+  </si>
+  <si>
+    <t>Bilinski</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Chando</t>
+  </si>
+  <si>
+    <t>McStravick</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Wackes</t>
+  </si>
+  <si>
+    <t>CHFC</t>
+  </si>
+  <si>
+    <t>** not on roster</t>
+  </si>
+  <si>
+    <t>Papperman</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -393,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +331,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,9 +362,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +678,7 @@
         <v>2020</v>
       </c>
       <c r="E1" s="2">
-        <v>43890</v>
+        <v>43892</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,7 +697,7 @@
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -774,6 +711,9 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -846,10 +786,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -857,10 +797,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -868,21 +808,21 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -890,46 +830,49 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
+      <c r="A15" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
+      <c r="A17" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -937,32 +880,32 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
@@ -970,10 +913,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
@@ -981,10 +924,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>8</v>
@@ -992,10 +935,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -1003,32 +946,32 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>114</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>49</v>
+      <c r="A26" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>8</v>
@@ -1036,10 +979,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
@@ -1047,10 +990,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>8</v>
@@ -1058,10 +1001,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>8</v>
@@ -1069,13 +1012,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
@@ -1083,10 +1023,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>8</v>
@@ -1094,367 +1034,187 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B47" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>106</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>93</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>95</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>113</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D64" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0305 Coaches Suspension Updated
</commit_message>
<xml_diff>
--- a/site/assets/Spring 2020 Coach Suspensions.xlsx
+++ b/site/assets/Spring 2020 Coach Suspensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
   <si>
     <t>suspended</t>
   </si>
@@ -107,12 +107,6 @@
     <t>Chris</t>
   </si>
   <si>
-    <t>Carroll</t>
-  </si>
-  <si>
-    <t>Jason</t>
-  </si>
-  <si>
     <t>Choilan</t>
   </si>
   <si>
@@ -179,18 +173,6 @@
     <t>Hirsch</t>
   </si>
   <si>
-    <t>Lisinski</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Marr</t>
-  </si>
-  <si>
-    <t>Kristin</t>
-  </si>
-  <si>
     <t>Paolone</t>
   </si>
   <si>
@@ -269,18 +251,9 @@
     <t>Jonathan</t>
   </si>
   <si>
-    <t>Kennedy</t>
-  </si>
-  <si>
     <t>Brogan</t>
   </si>
   <si>
-    <t>Bilinski</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
     <t>Chando</t>
   </si>
   <si>
@@ -303,9 +276,6 @@
   </si>
   <si>
     <t>Ryan</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
 </sst>
 </file>
@@ -648,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -786,10 +756,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -797,34 +767,37 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>82</v>
+      <c r="A12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>25</v>
+      <c r="A13" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -835,16 +808,16 @@
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
@@ -860,30 +833,27 @@
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -891,10 +861,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
@@ -902,32 +872,32 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>8</v>
@@ -935,21 +905,21 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>43</v>
+      <c r="A24" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -957,21 +927,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>8</v>
@@ -979,32 +949,33 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="1" t="s">
+    <row r="28" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>8</v>
@@ -1012,55 +983,57 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>8</v>
@@ -1068,35 +1041,33 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
@@ -1104,21 +1075,21 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1126,95 +1097,37 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>93</v>
+        <v>59</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>